<commit_message>
iniciando desduplicação rais estatística #2
</commit_message>
<xml_diff>
--- a/1files/layout_nomes.xlsx
+++ b/1files/layout_nomes.xlsx
@@ -4,17 +4,23 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
+    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Plan3!$A$1:$A$115</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Plan3!$A$1:$A$115</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="320">
   <si>
     <t>Conceito</t>
   </si>
@@ -314,16 +320,682 @@
   </si>
   <si>
     <t>RAIS_EST</t>
+  </si>
+  <si>
+    <t>RAIS_BRUTA</t>
+  </si>
+  <si>
+    <t>RAIS_EST_2</t>
+  </si>
+  <si>
+    <t>Ano Admissão</t>
+  </si>
+  <si>
+    <t>Causa Afastamento 1</t>
+  </si>
+  <si>
+    <t>Causa Afastamento 2</t>
+  </si>
+  <si>
+    <t>Causa Afastamento 3</t>
+  </si>
+  <si>
+    <t>CBO 94</t>
+  </si>
+  <si>
+    <t>CBO Ocupação 2002</t>
+  </si>
+  <si>
+    <t>CEI Vinculado</t>
+  </si>
+  <si>
+    <t>CNAE 2.0 Classe</t>
+  </si>
+  <si>
+    <t>CNAE 2.0 Subclasse</t>
+  </si>
+  <si>
+    <t>CNAE 95 Classe</t>
+  </si>
+  <si>
+    <t>CNPJ / CEI</t>
+  </si>
+  <si>
+    <t>CNPJ Contr Assist</t>
+  </si>
+  <si>
+    <t>CNPJ Contr Assoc</t>
+  </si>
+  <si>
+    <t>CNPJ Contr Assoc2</t>
+  </si>
+  <si>
+    <t>CNPJ Contr Conf</t>
+  </si>
+  <si>
+    <t>CNPJ Contr Sindical</t>
+  </si>
+  <si>
+    <t>CNPJ Raiz</t>
+  </si>
+  <si>
+    <t>CPF</t>
+  </si>
+  <si>
+    <t>Data Admissão Declarada</t>
+  </si>
+  <si>
+    <t>Data de Nascimento</t>
+  </si>
+  <si>
+    <t>Dia de Desligamento</t>
+  </si>
+  <si>
+    <t>Dia Fim AF1</t>
+  </si>
+  <si>
+    <t>Dia Fim AF2</t>
+  </si>
+  <si>
+    <t>Dia Fim AF3</t>
+  </si>
+  <si>
+    <t>Dia Ini AF1</t>
+  </si>
+  <si>
+    <t>Dia Ini AF2</t>
+  </si>
+  <si>
+    <t>Dia Ini AF3</t>
+  </si>
+  <si>
+    <t>Escolaridade após 2005</t>
+  </si>
+  <si>
+    <t>IBGE Subatividade</t>
+  </si>
+  <si>
+    <t>IBGE Subsetor</t>
+  </si>
+  <si>
+    <t>Idade</t>
+  </si>
+  <si>
+    <t>Ind Estab Participa PAT</t>
+  </si>
+  <si>
+    <t>Ind Hora Extra</t>
+  </si>
+  <si>
+    <t>Ind Portador Defic</t>
+  </si>
+  <si>
+    <t>Ind Simples</t>
+  </si>
+  <si>
+    <t>Ind Sindical</t>
+  </si>
+  <si>
+    <t>Ind Trab Intermitente</t>
+  </si>
+  <si>
+    <t>Ind Trab Parcial</t>
+  </si>
+  <si>
+    <t>Ind Trab Teletrabalho</t>
+  </si>
+  <si>
+    <t>Ind Vínculo Alvará</t>
+  </si>
+  <si>
+    <t>Mês Adiantamento 13º Salário</t>
+  </si>
+  <si>
+    <t>Mês Admissão</t>
+  </si>
+  <si>
+    <t>Mês Complemento 13º Salário</t>
+  </si>
+  <si>
+    <t>Mês Desligamento</t>
+  </si>
+  <si>
+    <t>Mês Fim AF1</t>
+  </si>
+  <si>
+    <t>Mês Fim AF2</t>
+  </si>
+  <si>
+    <t>Mês Fim AF3</t>
+  </si>
+  <si>
+    <t>Mês Ini AF1</t>
+  </si>
+  <si>
+    <t>Mês Ini AF2</t>
+  </si>
+  <si>
+    <t>Mês Ini AF3</t>
+  </si>
+  <si>
+    <t>Motivo Desligamento</t>
+  </si>
+  <si>
+    <t>Mun Trab</t>
+  </si>
+  <si>
+    <t>Município</t>
+  </si>
+  <si>
+    <t>Nacionalidade</t>
+  </si>
+  <si>
+    <t>Nome Trabalhador</t>
+  </si>
+  <si>
+    <t>Número CTPS</t>
+  </si>
+  <si>
+    <t>Qtd Dias Afastamento</t>
+  </si>
+  <si>
+    <t>Qtd Hora Contr</t>
+  </si>
+  <si>
+    <t>Qtd Hora Extra - Abril</t>
+  </si>
+  <si>
+    <t>Qtd Hora Extra - Agosto</t>
+  </si>
+  <si>
+    <t>Qtd Hora Extra - Dezembro</t>
+  </si>
+  <si>
+    <t>Qtd Hora Extra - Fevereiro</t>
+  </si>
+  <si>
+    <t>Qtd Hora Extra - Janeiro</t>
+  </si>
+  <si>
+    <t>Qtd Hora Extra - Julho</t>
+  </si>
+  <si>
+    <t>Qtd Hora Extra - Junho</t>
+  </si>
+  <si>
+    <t>Qtd Hora Extra - Maio</t>
+  </si>
+  <si>
+    <t>Qtd Hora Extra - Março</t>
+  </si>
+  <si>
+    <t>Qtd Hora Extra - Novembro</t>
+  </si>
+  <si>
+    <t>Qtd Hora Extra - Outubro</t>
+  </si>
+  <si>
+    <t>Qtd Hora Extra - Setembro</t>
+  </si>
+  <si>
+    <t>Qtd Meses Gratificação</t>
+  </si>
+  <si>
+    <t>Qtd Meses Hora Extra</t>
+  </si>
+  <si>
+    <t>Qtd Meses Reajuste Coletivo</t>
+  </si>
+  <si>
+    <t>Raça Cor</t>
+  </si>
+  <si>
+    <t>Sexo Trabalhador</t>
+  </si>
+  <si>
+    <t>Tempo Emprego</t>
+  </si>
+  <si>
+    <t>Tipo Admissão</t>
+  </si>
+  <si>
+    <t>Tipo Defic</t>
+  </si>
+  <si>
+    <t>Tipo Estab</t>
+  </si>
+  <si>
+    <t>Tipo Salário</t>
+  </si>
+  <si>
+    <t>Tipo Vínculo</t>
+  </si>
+  <si>
+    <t>Vínculo Ativo 31/12</t>
+  </si>
+  <si>
+    <t>Vl Adiantamento 13º Salário</t>
+  </si>
+  <si>
+    <t>Vl Complemento 13º  Salário</t>
+  </si>
+  <si>
+    <t>Vl Contr Assist</t>
+  </si>
+  <si>
+    <t>Vl Contr Assoc 1</t>
+  </si>
+  <si>
+    <t>Vl Contr Assoc 2</t>
+  </si>
+  <si>
+    <t>Vl Contr Conf</t>
+  </si>
+  <si>
+    <t>Vl Contr Sind</t>
+  </si>
+  <si>
+    <t>Vl Férias Venc Propor</t>
+  </si>
+  <si>
+    <t>Vl Gratificação</t>
+  </si>
+  <si>
+    <t>Vl Hora Extra</t>
+  </si>
+  <si>
+    <t>Vl Multa Rescisória</t>
+  </si>
+  <si>
+    <t>Vl Reajuste Coletivo</t>
+  </si>
+  <si>
+    <t>Vl Rem Abril CC</t>
+  </si>
+  <si>
+    <t>Vl Rem Agosto CC</t>
+  </si>
+  <si>
+    <t>Vl Rem Dezembro CC</t>
+  </si>
+  <si>
+    <t>Vl Rem Fevereiro CC</t>
+  </si>
+  <si>
+    <t>Vl Rem Janeiro CC</t>
+  </si>
+  <si>
+    <t>Vl Rem Julho CC</t>
+  </si>
+  <si>
+    <t>Vl Rem Junho CC</t>
+  </si>
+  <si>
+    <t>Vl Rem Maio CC</t>
+  </si>
+  <si>
+    <t>Vl Rem Março CC</t>
+  </si>
+  <si>
+    <t>Vl Rem Novembro CC</t>
+  </si>
+  <si>
+    <t>Vl Rem Outubro CC</t>
+  </si>
+  <si>
+    <t>Vl Rem Setembro CC</t>
+  </si>
+  <si>
+    <t>Vl Remun Dezembro (SM)</t>
+  </si>
+  <si>
+    <t>Vl Remun Dezembro Nom</t>
+  </si>
+  <si>
+    <t>Vl Remun Média (SM)</t>
+  </si>
+  <si>
+    <t>Vl Remun Média Nom</t>
+  </si>
+  <si>
+    <t>Vl Salário Contratual</t>
+  </si>
+  <si>
+    <t>Vl Última Remuneração Ano</t>
+  </si>
+  <si>
+    <t>data_desligamento</t>
+  </si>
+  <si>
+    <t>nome_var_padrao</t>
+  </si>
+  <si>
+    <t>CO_MOTIVO_SEGU_AFAS</t>
+  </si>
+  <si>
+    <t>CO_MOTIVO_TERC_AFAS</t>
+  </si>
+  <si>
+    <t>DA_FINAL_PRIMEIRO_AFAS</t>
+  </si>
+  <si>
+    <t>DA_FINAL_SEGUNDO_AFAS</t>
+  </si>
+  <si>
+    <t>DA_FINAL_TERCEIRO_AFAS</t>
+  </si>
+  <si>
+    <t>DA_INICIO_PRIMEIRO_AFAS</t>
+  </si>
+  <si>
+    <t>DA_INICIO_SEGUNDO_AFAS</t>
+  </si>
+  <si>
+    <t>DA_INICIO_TERCEIRO_AFAS</t>
+  </si>
+  <si>
+    <t>QT_DIAS_AFAS</t>
+  </si>
+  <si>
+    <t>AN_CHEGADA_RAIS</t>
+  </si>
+  <si>
+    <t>DA_NASCIMENTO_RAIS_DMA</t>
+  </si>
+  <si>
+    <t>IN_DEFICIENTE</t>
+  </si>
+  <si>
+    <t>CO_CPF</t>
+  </si>
+  <si>
+    <t>CO_CTPS_NUMERO</t>
+  </si>
+  <si>
+    <t>CO_CTPS_SERIE</t>
+  </si>
+  <si>
+    <t>CO_PIS_INFO</t>
+  </si>
+  <si>
+    <t>IN_ADMI_CONT_PIS_PASEP</t>
+  </si>
+  <si>
+    <t>IN_CODIGO_PIS_VALIDO</t>
+  </si>
+  <si>
+    <t>NO_PARTIC_RAIS</t>
+  </si>
+  <si>
+    <t>CO_CNPJ_CEI</t>
+  </si>
+  <si>
+    <t>CO_MUNICIPIO_LOCAL_TRABALHO</t>
+  </si>
+  <si>
+    <t>CO_TIPO_INSC_ESTAB_RAIS</t>
+  </si>
+  <si>
+    <t>CO_CNAE_SRF</t>
+  </si>
+  <si>
+    <t>QT_VINCULO_ESTAB</t>
+  </si>
+  <si>
+    <t>QT_VINCULO_ESTAB_ANT</t>
+  </si>
+  <si>
+    <t>AN_CADASTRAMENTO_PARTIC</t>
+  </si>
+  <si>
+    <t>DA_ADMISSAO_RAIS_DMA</t>
+  </si>
+  <si>
+    <t>DA_DESLIGAMENTO_RAIS_MD</t>
+  </si>
+  <si>
+    <t>TE_MES_TRABALHADO_CALC</t>
+  </si>
+  <si>
+    <t>QT_COMPETENCIA_BANC_HORA</t>
+  </si>
+  <si>
+    <t>QT_HORA_EXTR_TRAB_ABR</t>
+  </si>
+  <si>
+    <t>QT_HORA_EXTR_TRAB_AGO</t>
+  </si>
+  <si>
+    <t>QT_HORA_EXTR_TRAB_DEZ</t>
+  </si>
+  <si>
+    <t>QT_HORA_EXTR_TRAB_FEV</t>
+  </si>
+  <si>
+    <t>QT_HORA_EXTR_TRAB_JAN</t>
+  </si>
+  <si>
+    <t>QT_HORA_EXTR_TRAB_JUL</t>
+  </si>
+  <si>
+    <t>QT_HORA_EXTR_TRAB_JUN</t>
+  </si>
+  <si>
+    <t>QT_HORA_EXTR_TRAB_MAI</t>
+  </si>
+  <si>
+    <t>QT_HORA_EXTR_TRAB_MAR</t>
+  </si>
+  <si>
+    <t>QT_HORA_EXTR_TRAB_NOV</t>
+  </si>
+  <si>
+    <t>QT_HORA_EXTR_TRAB_OUT</t>
+  </si>
+  <si>
+    <t>QT_HORA_EXTR_TRAB_SET</t>
+  </si>
+  <si>
+    <t>CN_NUMERO_SEQ</t>
+  </si>
+  <si>
+    <t>IN_REMU_DEZ_RAIS_ANT</t>
+  </si>
+  <si>
+    <t>QT_COMPETENCIA_OUTR_GRAT</t>
+  </si>
+  <si>
+    <t>QT_MEDIA_SALARIO_MINIMO_ANO</t>
+  </si>
+  <si>
+    <t>QT_SALARIO_MINIMO_ANO</t>
+  </si>
+  <si>
+    <t>VA_OUTRAS_GRATIFICACOES</t>
+  </si>
+  <si>
+    <t>VA_REMU_DEZ_RAIS_ANT</t>
+  </si>
+  <si>
+    <t>VA_REMUNERACAO_ABR_RAIS</t>
+  </si>
+  <si>
+    <t>VA_REMUNERACAO_AGO_RAIS</t>
+  </si>
+  <si>
+    <t>VA_REMUNERACAO_FEV_RAIS</t>
+  </si>
+  <si>
+    <t>VA_REMUNERACAO_JAN_RAIS</t>
+  </si>
+  <si>
+    <t>VA_REMUNERACAO_JUL_RAIS</t>
+  </si>
+  <si>
+    <t>VA_REMUNERACAO_JUN_RAIS</t>
+  </si>
+  <si>
+    <t>VA_REMUNERACAO_MAI_RAIS</t>
+  </si>
+  <si>
+    <t>VA_REMUNERACAO_MAR_RAIS</t>
+  </si>
+  <si>
+    <t>VA_REMUNERACAO_NOV_RAIS</t>
+  </si>
+  <si>
+    <t>VA_REMUNERACAO_OUT_RAIS</t>
+  </si>
+  <si>
+    <t>VA_REMUNERACAO_SET_RAIS</t>
+  </si>
+  <si>
+    <t>VA_SALARIO_CONT_RAIS</t>
+  </si>
+  <si>
+    <t>CO_DATA_BASE</t>
+  </si>
+  <si>
+    <t>CO_TIPO_SALARIO_RAIS</t>
+  </si>
+  <si>
+    <t>IN_GRAVIDEZ</t>
+  </si>
+  <si>
+    <t>IN_RETIFICACAO_VINCULO</t>
+  </si>
+  <si>
+    <t>IN_SINDICALIZADO</t>
+  </si>
+  <si>
+    <t>IN_TELETRABALHO</t>
+  </si>
+  <si>
+    <t>IN_TRABALHOINTERMITENTE</t>
+  </si>
+  <si>
+    <t>IN_TRABALHOPARCIAL</t>
+  </si>
+  <si>
+    <t>CO_CNPJ_SIND_TRAB_BENE_ASSI</t>
+  </si>
+  <si>
+    <t>CO_CNPJ_SIND_TRAB_BENE_CA_1</t>
+  </si>
+  <si>
+    <t>CO_CNPJ_SIND_TRAB_BENE_CA_2</t>
+  </si>
+  <si>
+    <t>CO_CNPJ_SIND_TRAB_BENE_CONF</t>
+  </si>
+  <si>
+    <t>CO_CNPJ_SIND_TRAB_BENE_CS</t>
+  </si>
+  <si>
+    <t>CO_CREA</t>
+  </si>
+  <si>
+    <t>CO_DIAGNOSTICO_REG_RAIS</t>
+  </si>
+  <si>
+    <t>CO_UTILIZACAO_DADO_APOIO</t>
+  </si>
+  <si>
+    <t>IN_ALVARA_JUDICIAL</t>
+  </si>
+  <si>
+    <t>IN_ANTECIPADO</t>
+  </si>
+  <si>
+    <t>ME_13SA</t>
+  </si>
+  <si>
+    <t>ME_13SF</t>
+  </si>
+  <si>
+    <t>nchars</t>
+  </si>
+  <si>
+    <t>ncharslayout</t>
+  </si>
+  <si>
+    <t>VA_13SA</t>
+  </si>
+  <si>
+    <t>VA_13SF</t>
+  </si>
+  <si>
+    <t>VA_AVISO_PREVIO_INDENIZADO</t>
+  </si>
+  <si>
+    <t>VA_REPA_SIND_TRAB_BENE_ASSI</t>
+  </si>
+  <si>
+    <t>VA_REPA_SIND_TRAB_BENE_CA_1</t>
+  </si>
+  <si>
+    <t>VA_REPA_SIND_TRAB_BENE_CA_2</t>
+  </si>
+  <si>
+    <t>VA_REPA_SIND_TRAB_BENE_CONF</t>
+  </si>
+  <si>
+    <t>VA_REPA_SIND_TRAB_BENE_CS</t>
+  </si>
+  <si>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t>xxxx</t>
+  </si>
+  <si>
+    <t>AN</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>DA</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>nc</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>QT</t>
+  </si>
+  <si>
+    <t>TE</t>
+  </si>
+  <si>
+    <t>VA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -413,7 +1085,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -428,6 +1100,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -733,10 +1412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="D48" sqref="D1:D1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,19 +1426,24 @@
     <col min="4" max="4" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>99</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="D1" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -773,7 +1457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -785,7 +1469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -797,7 +1481,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
@@ -809,7 +1493,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
@@ -821,7 +1505,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
@@ -833,7 +1517,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
@@ -845,7 +1529,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -857,7 +1541,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -871,7 +1555,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>14</v>
       </c>
@@ -883,7 +1567,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>15</v>
       </c>
@@ -895,7 +1579,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
@@ -907,7 +1591,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>17</v>
       </c>
@@ -919,7 +1603,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>18</v>
       </c>
@@ -931,7 +1615,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
@@ -1504,4 +2188,2149 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B117"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="9" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="9" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="9" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C115"/>
+  <sheetViews>
+    <sheetView topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="A118" sqref="A118"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C2" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C3" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B4" t="s">
+        <v>310</v>
+      </c>
+      <c r="C4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
+        <v>311</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B6" t="s">
+        <v>311</v>
+      </c>
+      <c r="C6" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B7" t="s">
+        <v>311</v>
+      </c>
+      <c r="C7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>311</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>311</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>311</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
+        <v>311</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
+        <v>311</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B13" t="s">
+        <v>311</v>
+      </c>
+      <c r="C13" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B14" t="s">
+        <v>311</v>
+      </c>
+      <c r="C14" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B15" t="s">
+        <v>311</v>
+      </c>
+      <c r="C15" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>311</v>
+      </c>
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B17" t="s">
+        <v>311</v>
+      </c>
+      <c r="C17" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B18" t="s">
+        <v>311</v>
+      </c>
+      <c r="C18" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>311</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B20" t="s">
+        <v>311</v>
+      </c>
+      <c r="C20" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
+        <v>311</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>311</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B23" t="s">
+        <v>311</v>
+      </c>
+      <c r="C23" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B24" t="s">
+        <v>311</v>
+      </c>
+      <c r="C24" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>311</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" t="s">
+        <v>311</v>
+      </c>
+      <c r="C26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" t="s">
+        <v>311</v>
+      </c>
+      <c r="C27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" t="s">
+        <v>311</v>
+      </c>
+      <c r="C28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" t="s">
+        <v>311</v>
+      </c>
+      <c r="C29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B30" t="s">
+        <v>311</v>
+      </c>
+      <c r="C30" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B31" t="s">
+        <v>311</v>
+      </c>
+      <c r="C31" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B32" t="s">
+        <v>311</v>
+      </c>
+      <c r="C32" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B33" t="s">
+        <v>311</v>
+      </c>
+      <c r="C33" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B34" t="s">
+        <v>311</v>
+      </c>
+      <c r="C34" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B35" t="s">
+        <v>311</v>
+      </c>
+      <c r="C35" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B36" t="s">
+        <v>311</v>
+      </c>
+      <c r="C36" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B37" t="s">
+        <v>311</v>
+      </c>
+      <c r="C37" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B38" t="s">
+        <v>311</v>
+      </c>
+      <c r="C38" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B39" t="s">
+        <v>311</v>
+      </c>
+      <c r="C39" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B40" t="s">
+        <v>312</v>
+      </c>
+      <c r="C40" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B41" t="s">
+        <v>312</v>
+      </c>
+      <c r="C41" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B42" t="s">
+        <v>312</v>
+      </c>
+      <c r="C42" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B43" t="s">
+        <v>312</v>
+      </c>
+      <c r="C43" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B44" t="s">
+        <v>312</v>
+      </c>
+      <c r="C44" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B45" t="s">
+        <v>312</v>
+      </c>
+      <c r="C45" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B46" t="s">
+        <v>312</v>
+      </c>
+      <c r="C46" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B47" t="s">
+        <v>312</v>
+      </c>
+      <c r="C47" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B48" t="s">
+        <v>312</v>
+      </c>
+      <c r="C48" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B49" t="s">
+        <v>313</v>
+      </c>
+      <c r="C49" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B50" t="s">
+        <v>313</v>
+      </c>
+      <c r="C50" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B51" t="s">
+        <v>313</v>
+      </c>
+      <c r="C51" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52" t="s">
+        <v>313</v>
+      </c>
+      <c r="C52" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B53" t="s">
+        <v>313</v>
+      </c>
+      <c r="C53" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B54" t="s">
+        <v>313</v>
+      </c>
+      <c r="C54" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B55" t="s">
+        <v>313</v>
+      </c>
+      <c r="C55" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B56" t="s">
+        <v>313</v>
+      </c>
+      <c r="C56" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B57" t="s">
+        <v>313</v>
+      </c>
+      <c r="C57" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B58" t="s">
+        <v>313</v>
+      </c>
+      <c r="C58" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B59" t="s">
+        <v>313</v>
+      </c>
+      <c r="C59" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B60" t="s">
+        <v>313</v>
+      </c>
+      <c r="C60" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B61" t="s">
+        <v>313</v>
+      </c>
+      <c r="C61" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B62" t="s">
+        <v>314</v>
+      </c>
+      <c r="C62" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B63" t="s">
+        <v>314</v>
+      </c>
+      <c r="C63" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B64" t="s">
+        <v>315</v>
+      </c>
+      <c r="C64" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B65" t="s">
+        <v>315</v>
+      </c>
+      <c r="C65" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B66" t="s">
+        <v>316</v>
+      </c>
+      <c r="C66" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B67" t="s">
+        <v>317</v>
+      </c>
+      <c r="C67" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B68" t="s">
+        <v>317</v>
+      </c>
+      <c r="C68" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B69" t="s">
+        <v>317</v>
+      </c>
+      <c r="C69" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B70" t="s">
+        <v>317</v>
+      </c>
+      <c r="C70" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B71" t="s">
+        <v>317</v>
+      </c>
+      <c r="C71" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B72" t="s">
+        <v>317</v>
+      </c>
+      <c r="C72" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B73" t="s">
+        <v>317</v>
+      </c>
+      <c r="C73" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B74" t="s">
+        <v>317</v>
+      </c>
+      <c r="C74" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B75" t="s">
+        <v>317</v>
+      </c>
+      <c r="C75" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B76" t="s">
+        <v>317</v>
+      </c>
+      <c r="C76" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B77" t="s">
+        <v>317</v>
+      </c>
+      <c r="C77" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B78" t="s">
+        <v>317</v>
+      </c>
+      <c r="C78" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B79" t="s">
+        <v>317</v>
+      </c>
+      <c r="C79" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B80" t="s">
+        <v>317</v>
+      </c>
+      <c r="C80" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B81" t="s">
+        <v>317</v>
+      </c>
+      <c r="C81" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B82" t="s">
+        <v>317</v>
+      </c>
+      <c r="C82" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B83" t="s">
+        <v>317</v>
+      </c>
+      <c r="C83" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B84" t="s">
+        <v>317</v>
+      </c>
+      <c r="C84" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B85" t="s">
+        <v>317</v>
+      </c>
+      <c r="C85" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B86" t="s">
+        <v>317</v>
+      </c>
+      <c r="C86" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B87" t="s">
+        <v>317</v>
+      </c>
+      <c r="C87" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B88" t="s">
+        <v>318</v>
+      </c>
+      <c r="C88" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B89" t="s">
+        <v>319</v>
+      </c>
+      <c r="C89" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B90" t="s">
+        <v>319</v>
+      </c>
+      <c r="C90" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B91" t="s">
+        <v>319</v>
+      </c>
+      <c r="C91" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B92" t="s">
+        <v>319</v>
+      </c>
+      <c r="C92" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B93" t="s">
+        <v>319</v>
+      </c>
+      <c r="C93" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B94" t="s">
+        <v>319</v>
+      </c>
+      <c r="C94" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B95" t="s">
+        <v>319</v>
+      </c>
+      <c r="C95" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B96" t="s">
+        <v>319</v>
+      </c>
+      <c r="C96" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B97" t="s">
+        <v>319</v>
+      </c>
+      <c r="C97" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B98" t="s">
+        <v>319</v>
+      </c>
+      <c r="C98" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B99" t="s">
+        <v>319</v>
+      </c>
+      <c r="C99" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B100" t="s">
+        <v>319</v>
+      </c>
+      <c r="C100" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B101" t="s">
+        <v>319</v>
+      </c>
+      <c r="C101" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B102" t="s">
+        <v>319</v>
+      </c>
+      <c r="C102" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B103" t="s">
+        <v>319</v>
+      </c>
+      <c r="C103" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B104" t="s">
+        <v>319</v>
+      </c>
+      <c r="C104" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B105" t="s">
+        <v>319</v>
+      </c>
+      <c r="C105" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B106" t="s">
+        <v>319</v>
+      </c>
+      <c r="C106" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B107" t="s">
+        <v>319</v>
+      </c>
+      <c r="C107" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B108" t="s">
+        <v>319</v>
+      </c>
+      <c r="C108" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B109" t="s">
+        <v>319</v>
+      </c>
+      <c r="C109" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B110" t="s">
+        <v>319</v>
+      </c>
+      <c r="C110" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B111" t="s">
+        <v>319</v>
+      </c>
+      <c r="C111" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B112" t="s">
+        <v>319</v>
+      </c>
+      <c r="C112" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B113" t="s">
+        <v>319</v>
+      </c>
+      <c r="C113" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B114" t="s">
+        <v>319</v>
+      </c>
+      <c r="C114" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B115" t="s">
+        <v>319</v>
+      </c>
+      <c r="C115" t="s">
+        <v>306</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>